<commit_message>
updated figures 5 and 6
</commit_message>
<xml_diff>
--- a/AC_age_EIA.xlsx
+++ b/AC_age_EIA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbiscoch/Documents/Research_remote/GitHub/hp_proj1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbiscoch/Documents/Research_remote/GitHub/Comparing-Top-Down-Heat-Pump-Energy-Consumption-with-Measured-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26A276B-EB9A-8B4A-B068-1AAEDB54974E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5172B68C-7B82-2745-BE68-88123F9D1586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{DF4E7D9B-ECD9-B549-AE16-1A5C62463C83}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="2010" sheetId="1" r:id="rId1"/>
     <sheet name="2020" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,9 +45,6 @@
     <t>Year of purchase, central AC</t>
   </si>
   <si>
-    <t>(2007-2009]</t>
-  </si>
-  <si>
     <t>[2005, 2007]</t>
   </si>
   <si>
@@ -75,7 +72,10 @@
     <t>Main AC Units purchased before 2006</t>
   </si>
   <si>
-    <t>Main AC Units purchased after 2006</t>
+    <t>[2008-2009]</t>
+  </si>
+  <si>
+    <t>Main AC Units purchased after the start of 2006 but before the end of 2010</t>
   </si>
 </sst>
 </file>
@@ -118,10 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -439,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C82537D-A66D-5C4A-801C-37D88A3D8233}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,13 +451,12 @@
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -466,87 +464,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <f>3.2+3+1.4+1.2</f>
         <v>8.7999999999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <f>1.4+0.6+0.3+0.3</f>
         <v>2.5999999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
       </c>
       <c r="B13">
         <f>SUM(B3,B8)</f>
         <v>1.2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <f>SUM(B4,B9)</f>
         <v>2.5999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <f>SUM(B5,B10)</f>
@@ -558,12 +556,12 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>3.4</v>
@@ -571,12 +569,12 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>1.6</v>
@@ -584,12 +582,12 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <f>SUM(B18,B21)</f>
@@ -598,20 +596,20 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26">
-        <f>B15+B14/2</f>
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+        <f>B15+B14*(1/3)</f>
+        <v>12.266666666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B27">
-        <f>B14/2+B13+B24/4</f>
-        <v>3.75</v>
+        <f>B14*2/3+B13+B24/5</f>
+        <v>3.9333333333333331</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>